<commit_message>
Boton de ayuda, y se agrega validacion solo texto y se corrige las validaciones
</commit_message>
<xml_diff>
--- a/CAC Artritis (copia).xlsx
+++ b/CAC Artritis (copia).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="166">
   <si>
     <t xml:space="preserve">1. Código de la EAPB o de la entidad territorial</t>
   </si>
@@ -494,28 +494,34 @@
     <t xml:space="preserve">NONE</t>
   </si>
   <si>
+    <t xml:space="preserve">sdhfsjh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1977/11/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL 13 CRA 18  # 17-18. B. FLORIDA MAGANGUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1799-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">050010412701</t>
+  </si>
+  <si>
     <t xml:space="preserve">hghgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1977/11/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL 13 CRA 18  # 17-18. B. FLORIDA MAGANGUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1799-01-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">050010412701</t>
   </si>
   <si>
     <t xml:space="preserve">20150930_RES002_ARTRITIS.txt</t>
@@ -889,77 +895,77 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="EV1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="EV3" activeCellId="0" sqref="EV3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="39.2064777327935"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="113.331983805668"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="48.8461538461539"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="78.3036437246964"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="25" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="43" min="32" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="54.7368421052632"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="50" min="47" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="119.546558704453"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="51.2024291497976"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="25" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="43" min="32" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="50" min="47" style="0" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="73" min="54" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="77" min="74" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="80" min="79" style="0" width="61.5951417004049"/>
-    <col collapsed="false" hidden="false" max="88" min="81" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="94" min="89" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="97" min="97" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="51.6315789473684"/>
-    <col collapsed="false" hidden="false" max="102" min="101" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="77" min="74" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="80" min="79" style="0" width="64.8056680161943"/>
+    <col collapsed="false" hidden="false" max="88" min="81" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="94" min="89" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="97" min="97" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="102" min="101" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="104" min="103" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="107" min="106" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="54.7368421052632"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="128" min="109" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="132" min="129" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="135" min="133" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="132" min="129" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="135" min="133" style="0" width="59.4493927125506"/>
     <col collapsed="false" hidden="false" max="139" min="136" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="140" min="140" style="0" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="144" min="144" style="0" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="47.2388663967611"/>
-    <col collapsed="false" hidden="false" max="147" min="147" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="148" min="148" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="149" min="149" style="1" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="150" min="150" style="1" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="151" min="151" style="0" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="152" min="152" style="1" width="68.7692307692308"/>
+    <col collapsed="false" hidden="false" max="140" min="140" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="63.7368421052632"/>
+    <col collapsed="false" hidden="false" max="144" min="144" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="147" min="147" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="148" min="148" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="149" min="149" style="1" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="150" min="150" style="1" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="151" min="151" style="0" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="152" min="152" style="1" width="72.5182186234818"/>
     <col collapsed="false" hidden="false" max="870" min="153" style="2" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="871" style="0" width="11.4615384615385"/>
   </cols>
@@ -1589,7 +1595,7 @@
       <c r="D2" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>155</v>
       </c>
       <c r="F2" s="16" t="s">
@@ -1626,7 +1632,7 @@
         <v>36935</v>
       </c>
       <c r="Q2" s="21" t="n">
-        <v>-36521</v>
+        <v>-32505</v>
       </c>
       <c r="R2" s="22" t="n">
         <v>36970</v>
@@ -1656,10 +1662,10 @@
         <v>1</v>
       </c>
       <c r="AA2" s="23" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="AB2" s="23" t="n">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="AC2" s="23" t="n">
         <v>0</v>
@@ -1718,8 +1724,8 @@
       <c r="AU2" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="AV2" s="23" t="n">
-        <v>1</v>
+      <c r="AV2" s="23" t="s">
+        <v>162</v>
       </c>
       <c r="AW2" s="23" t="n">
         <v>1</v>
@@ -1996,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="EJ2" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="EK2" s="25" t="n">
         <v>25148</v>
@@ -2032,7 +2038,7 @@
         <v>22427664</v>
       </c>
       <c r="EV2" s="16" t="n">
-        <v>0</v>
+        <v>178.21251</v>
       </c>
       <c r="AGM2" s="0"/>
       <c r="AGN2" s="0"/>
@@ -2203,7 +2209,7 @@
         <v>154</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>154</v>
@@ -2609,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="EJ3" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="EK3" s="25" t="n">
         <v>25148</v>
@@ -3380,7 +3386,7 @@
         <v>154</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>154</v>
@@ -3786,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="EJ4" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="EK4" s="25" t="n">
         <v>25148</v>
@@ -5528,13 +5534,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="62.663967611336"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realizan ajustes de esteban, cambiar mayusculas, quitar espciaso, validacion del regimen, mostrar mensaje del cargue del archivo
</commit_message>
<xml_diff>
--- a/CAC Artritis (copia).xlsx
+++ b/CAC Artritis (copia).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="166">
   <si>
     <t xml:space="preserve">1. Código de la EAPB o de la entidad territorial</t>
   </si>
@@ -491,16 +491,19 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
+    <t xml:space="preserve"> jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdhfsjh </t>
+  </si>
+  <si>
     <t xml:space="preserve">NONE</t>
   </si>
   <si>
-    <t xml:space="preserve">sdhfsjh </t>
-  </si>
-  <si>
     <t xml:space="preserve">CC</t>
   </si>
   <si>
-    <t xml:space="preserve">1977/11/17</t>
+    <t xml:space="preserve"> 10.08.1986</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
@@ -513,9 +516,6 @@
   </si>
   <si>
     <t xml:space="preserve">1799-01-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r</t>
   </si>
   <si>
     <t xml:space="preserve">050010412701</t>
@@ -895,79 +895,79 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AV2" activeCellId="0" sqref="AV2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="121.793522267206"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="52.0607287449393"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="83.8744939271255"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="28" min="25" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="41.2388663967611"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="43" min="32" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="50" min="47" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="46.5951417004049"/>
-    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="73" min="54" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="77" min="74" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="58.0566801619433"/>
-    <col collapsed="false" hidden="false" max="80" min="79" style="0" width="65.8785425101215"/>
-    <col collapsed="false" hidden="false" max="88" min="81" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="94" min="89" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="97" min="97" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="55.2753036437247"/>
-    <col collapsed="false" hidden="false" max="102" min="101" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="104" min="103" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="107" min="106" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="128" min="109" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="132" min="129" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="135" min="133" style="0" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="139" min="136" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="140" min="140" style="0" width="53.4534412955466"/>
-    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="79.6963562753036"/>
-    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="64.8056680161943"/>
-    <col collapsed="false" hidden="false" max="144" min="144" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="50.3441295546559"/>
-    <col collapsed="false" hidden="false" max="147" min="147" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="148" min="148" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="149" min="149" style="1" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="150" min="150" style="1" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="151" min="151" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="152" min="152" style="1" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="870" min="153" style="2" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="871" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="111.367346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="76.4030612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="28" min="25" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="32" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="50" min="47" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="73" min="54" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="77" min="74" style="0" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="0" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="80" min="79" style="0" width="59.8010204081633"/>
+    <col collapsed="false" hidden="false" max="88" min="81" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="94" min="89" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="95" min="95" style="0" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="96" min="96" style="0" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="97" min="97" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="99" min="99" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="100" min="100" style="0" width="50.219387755102"/>
+    <col collapsed="false" hidden="false" max="102" min="101" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="104" min="103" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="105" min="105" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="107" min="106" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="128" min="109" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="132" min="129" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="135" min="133" style="0" width="54.9438775510204"/>
+    <col collapsed="false" hidden="false" max="139" min="136" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="140" min="140" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="141" min="141" style="0" width="72.7602040816327"/>
+    <col collapsed="false" hidden="false" max="142" min="142" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="143" min="143" style="0" width="58.9897959183674"/>
+    <col collapsed="false" hidden="false" max="144" min="144" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="145" min="145" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="146" min="146" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="147" min="147" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="148" min="148" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="149" min="149" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="150" min="150" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="151" min="151" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="152" min="152" style="1" width="67.0918367346939"/>
+    <col collapsed="false" hidden="false" max="870" min="153" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="871" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1590,7 +1590,7 @@
         <v>153</v>
       </c>
       <c r="C2" s="16" t="n">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>154</v>
@@ -1599,34 +1599,34 @@
         <v>155</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I2" s="16" t="n">
         <v>34534643</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L2" s="16" t="n">
         <v>6</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N2" s="18" t="n">
         <v>3145747676</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P2" s="20" t="n">
         <v>36935</v>
@@ -1638,7 +1638,7 @@
         <v>36970</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T2" s="23" t="n">
         <v>164</v>
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="AN2" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO2" s="23" t="n">
         <v>1</v>
@@ -1710,7 +1710,7 @@
         <v>300</v>
       </c>
       <c r="AQ2" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AR2" s="23" t="n">
         <v>300</v>
@@ -1724,14 +1724,14 @@
       <c r="AU2" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="AV2" s="23" t="s">
+      <c r="AV2" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="23" t="s">
         <v>162</v>
-      </c>
-      <c r="AW2" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="23" t="s">
-        <v>161</v>
       </c>
       <c r="AY2" s="23" t="n">
         <v>0</v>
@@ -1863,11 +1863,11 @@
         <v>1</v>
       </c>
       <c r="CP2" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CQ2" s="23" t="n">
         <f aca="false">IF(CP2&gt;J2,1,9)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="CR2" s="23" t="n">
         <v>6</v>
@@ -1876,7 +1876,7 @@
         <v>300</v>
       </c>
       <c r="CT2" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CU2" s="23" t="n">
         <v>300</v>
@@ -2008,7 +2008,7 @@
         <v>25148</v>
       </c>
       <c r="EL2" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EM2" s="23" t="n">
         <v>6</v>
@@ -2017,13 +2017,13 @@
         <v>0</v>
       </c>
       <c r="EO2" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EP2" s="23" t="n">
         <v>999999</v>
       </c>
       <c r="EQ2" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="ER2" s="23" t="n">
         <v>0</v>
@@ -2206,19 +2206,19 @@
         <v>99</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>164</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I3" s="16" t="n">
         <v>34534643</v>
@@ -2227,19 +2227,19 @@
         <v>28446</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L3" s="16" t="n">
         <v>6</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N3" s="18" t="n">
         <v>3145747676</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P3" s="20" t="n">
         <v>36935</v>
@@ -2251,7 +2251,7 @@
         <v>36970</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T3" s="23" t="n">
         <v>164</v>
@@ -2314,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="AN3" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO3" s="23" t="n">
         <v>1</v>
@@ -2323,7 +2323,7 @@
         <v>300</v>
       </c>
       <c r="AQ3" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AR3" s="23" t="n">
         <v>300</v>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="AX3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AY3" s="23" t="n">
         <v>0</v>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="CP3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CQ3" s="23" t="n">
         <f aca="false">IF(CP3&gt;J3,1,9)</f>
@@ -2489,7 +2489,7 @@
         <v>300</v>
       </c>
       <c r="CT3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CU3" s="23" t="n">
         <v>300</v>
@@ -2621,7 +2621,7 @@
         <v>25148</v>
       </c>
       <c r="EL3" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EM3" s="23" t="n">
         <v>6</v>
@@ -2630,13 +2630,13 @@
         <v>0</v>
       </c>
       <c r="EO3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EP3" s="23" t="n">
         <v>999999</v>
       </c>
       <c r="EQ3" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="ER3" s="23" t="n">
         <v>0</v>
@@ -3383,19 +3383,19 @@
         <v>99</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>164</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I4" s="16" t="n">
         <v>34534643</v>
@@ -3404,19 +3404,19 @@
         <v>28446</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L4" s="16" t="n">
         <v>6</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N4" s="18" t="n">
         <v>3145747676</v>
       </c>
       <c r="O4" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="P4" s="20" t="n">
         <v>36935</v>
@@ -3428,7 +3428,7 @@
         <v>36970</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T4" s="23" t="n">
         <v>164</v>
@@ -3491,7 +3491,7 @@
         <v>1</v>
       </c>
       <c r="AN4" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO4" s="23" t="n">
         <v>1</v>
@@ -3500,7 +3500,7 @@
         <v>300</v>
       </c>
       <c r="AQ4" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AR4" s="23" t="n">
         <v>300</v>
@@ -3521,7 +3521,7 @@
         <v>1</v>
       </c>
       <c r="AX4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AY4" s="23" t="n">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="CP4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CQ4" s="23" t="n">
         <f aca="false">IF(CP4&gt;J4,1,9)</f>
@@ -3666,7 +3666,7 @@
         <v>300</v>
       </c>
       <c r="CT4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="CU4" s="23" t="n">
         <v>300</v>
@@ -3798,7 +3798,7 @@
         <v>25148</v>
       </c>
       <c r="EL4" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EM4" s="23" t="n">
         <v>6</v>
@@ -3807,13 +3807,13 @@
         <v>0</v>
       </c>
       <c r="EO4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="EP4" s="23" t="n">
         <v>999999</v>
       </c>
       <c r="EQ4" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="ER4" s="23" t="n">
         <v>0</v>
@@ -5534,8 +5534,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>